<commit_message>
Reset migrations and add seed
</commit_message>
<xml_diff>
--- a/seed.xlsx
+++ b/seed.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UserFiles\desktop\ecole\WEB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\He-Arc\bullet-dynamics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605BEAA5-C602-4DC9-92A1-571BDDAB2007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D59967-BF59-448B-AFA9-312559B1A75D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35AEAFD1-6C6C-4E24-93C8-52E24EB07AEC}"/>
+    <workbookView xWindow="6390" yWindow="870" windowWidth="21600" windowHeight="11385" xr2:uid="{35AEAFD1-6C6C-4E24-93C8-52E24EB07AEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631A4EB9-E2D3-472E-8A96-90294C0319E2}">
   <dimension ref="A4:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>